<commit_message>
Adjust mental health values to increase effect size.
Signed-off-by: Hendriela <hendrik-heiser@gmx.de>
</commit_message>
<xml_diff>
--- a/src/data/ICHOM_PROM_breast_cancer_dummy_answers.xlsx
+++ b/src/data/ICHOM_PROM_breast_cancer_dummy_answers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hendrik\PycharmProjects\hackzurich2021\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4021BA13-4ECC-474E-A4CE-BF88B82B1B54}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B4213A-6C91-4055-8317-93C41BD50CC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -620,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2388,10 +2388,10 @@
         <v>2</v>
       </c>
       <c r="O45">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P45">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2429,10 +2429,10 @@
         <v>2</v>
       </c>
       <c r="O46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P46">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2467,13 +2467,13 @@
         <v>2</v>
       </c>
       <c r="N47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P47">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>